<commit_message>
Running DBSCAN on test cluster
Changing df0 in the DBSCAN notebook to the test cluster to demonstrate how the algorithm works.
</commit_message>
<xml_diff>
--- a/DataTables/TestParameters.xlsx
+++ b/DataTables/TestParameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/731fb941f3e8f028/Documents/GitHub/CraterClusterTools/DataTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="114_{FAB727D4-F300-4AD0-9251-68BC0DF9A6A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{17FB8DF5-A7DA-471C-9C6B-B18780F59262}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="114_{FAB727D4-F300-4AD0-9251-68BC0DF9A6A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D10FF4FB-719B-47FE-9631-7E88AC20175E}"/>
   <bookViews>
     <workbookView xWindow="1725" yWindow="1155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Dispersion</t>
   </si>
@@ -56,16 +56,13 @@
   </si>
   <si>
     <t>ESP_013694_2060</t>
-  </si>
-  <si>
-    <t>HiRiseID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +74,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,11 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,14 +430,14 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>12</v>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -513,5 +519,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>